<commit_message>
MAJ fonction informations compte / Planning / UserStories
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Completé</t>
   </si>
@@ -750,7 +750,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +881,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="7">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>2</v>
@@ -905,7 +905,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="7">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>2</v>
@@ -953,7 +953,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="7">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="20"/>
@@ -977,7 +977,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="20"/>
@@ -1001,7 +1001,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="8">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>2</v>
@@ -1010,7 +1010,9 @@
       <c r="E10" s="12"/>
       <c r="F10" s="24"/>
       <c r="G10" s="25"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="20"/>
       <c r="K10" s="6"/>
@@ -1025,14 +1027,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="8">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="20"/>
       <c r="E11" s="12"/>
       <c r="F11" s="24"/>
       <c r="G11" s="25"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="20"/>
       <c r="K11" s="6"/>
@@ -1047,14 +1051,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="20"/>
       <c r="E12" s="12"/>
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="20"/>
       <c r="K12" s="6"/>
@@ -1091,14 +1097,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="8">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="20"/>
       <c r="E14" s="12"/>
       <c r="F14" s="24"/>
       <c r="G14" s="25"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" s="20"/>
       <c r="K14" s="6"/>
@@ -1113,7 +1121,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="8">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="20"/>
@@ -1297,7 +1305,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="8">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>2</v>
@@ -1502,7 +1510,7 @@
       </c>
       <c r="B34" s="8">
         <f>AVERAGE(B9:B33)</f>
-        <v>0.13333333333333333</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="21"/>

</xml_diff>